<commit_message>
Actualizacion del avance del cronograma
</commit_message>
<xml_diff>
--- a/Desarrollo/SGDS/Gestion/SGDS - CP.XLS.xlsx
+++ b/Desarrollo/SGDS/Gestion/SGDS - CP.XLS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Backup\Escritorio\QuantumAnts Software\QuantumAnts-Software\Desarrollo\Gestion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Proyecto_Grupo_5\QuantumAnts-Software\Desarrollo\SGDS\Gestion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C897912-8345-49CD-B53F-A5628996DACD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7837725-E423-40CC-BDE0-3586418679EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cronograma #1" sheetId="1" r:id="rId1"/>
@@ -703,9 +703,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
-  </numFmts>
   <fonts count="50">
     <font>
       <sz val="10"/>
@@ -1470,7 +1467,7 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="8" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1497,7 +1494,7 @@
     <xf numFmtId="0" fontId="13" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="13" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="14" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1507,15 +1504,15 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="13" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="13" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="13" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="17" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="14" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="14" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1525,7 +1522,7 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="14" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="14" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1537,7 +1534,7 @@
     <xf numFmtId="0" fontId="19" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="20" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="21" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="14" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="14" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1546,7 +1543,7 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="24" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="24" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="8" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1557,7 +1554,7 @@
     <xf numFmtId="9" fontId="27" fillId="5" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1576,7 +1573,7 @@
     <xf numFmtId="0" fontId="30" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="31" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="31" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="30" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1595,7 +1592,7 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="8" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="30" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1678,6 +1675,7 @@
     <xf numFmtId="0" fontId="44" fillId="6" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1691,7 +1689,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -1913,8 +1910,8 @@
   </sheetPr>
   <dimension ref="A1:K998"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="C5" workbookViewId="0">
+      <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1"/>
@@ -1931,23 +1928,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="32.25" customHeight="1">
-      <c r="A1" s="112" t="s">
+      <c r="A1" s="113" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="111"/>
-      <c r="C1" s="111"/>
-      <c r="D1" s="111"/>
-      <c r="E1" s="111"/>
-      <c r="F1" s="111"/>
-      <c r="G1" s="111"/>
-      <c r="H1" s="111"/>
+      <c r="B1" s="112"/>
+      <c r="C1" s="112"/>
+      <c r="D1" s="112"/>
+      <c r="E1" s="112"/>
+      <c r="F1" s="112"/>
+      <c r="G1" s="112"/>
+      <c r="H1" s="112"/>
     </row>
     <row r="2" spans="1:11" ht="15.75" customHeight="1">
       <c r="A2" s="1"/>
-      <c r="B2" s="113" t="s">
+      <c r="B2" s="114" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="114"/>
+      <c r="C2" s="115"/>
       <c r="D2" s="2"/>
       <c r="E2" s="1"/>
       <c r="F2" s="3"/>
@@ -2005,7 +2002,7 @@
         <v>45022</v>
       </c>
       <c r="D6" s="2"/>
-      <c r="E6" s="117"/>
+      <c r="E6" s="110"/>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
       <c r="H6" s="4"/>
@@ -2137,7 +2134,7 @@
       <c r="H12" s="20">
         <v>1</v>
       </c>
-      <c r="I12" s="110" t="s">
+      <c r="I12" s="111" t="s">
         <v>25</v>
       </c>
       <c r="J12" s="2"/>
@@ -2166,7 +2163,7 @@
       <c r="H13" s="20">
         <v>1</v>
       </c>
-      <c r="I13" s="111"/>
+      <c r="I13" s="112"/>
       <c r="J13" s="2"/>
     </row>
     <row r="14" spans="1:11" ht="15.75" customHeight="1" thickBot="1">
@@ -2192,7 +2189,7 @@
       <c r="H14" s="20">
         <v>1</v>
       </c>
-      <c r="I14" s="111"/>
+      <c r="I14" s="112"/>
       <c r="J14" s="2"/>
     </row>
     <row r="15" spans="1:11" ht="15.75" customHeight="1" thickBot="1">
@@ -2218,7 +2215,7 @@
       <c r="H15" s="20">
         <v>1</v>
       </c>
-      <c r="I15" s="111"/>
+      <c r="I15" s="112"/>
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
     </row>
@@ -2245,7 +2242,7 @@
       <c r="H16" s="20">
         <v>1</v>
       </c>
-      <c r="I16" s="111"/>
+      <c r="I16" s="112"/>
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
     </row>
@@ -2272,7 +2269,7 @@
       <c r="H17" s="20">
         <v>1</v>
       </c>
-      <c r="I17" s="111"/>
+      <c r="I17" s="112"/>
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
     </row>
@@ -2299,7 +2296,7 @@
       <c r="H18" s="20">
         <v>1</v>
       </c>
-      <c r="I18" s="111"/>
+      <c r="I18" s="112"/>
       <c r="J18" s="2"/>
       <c r="K18" s="2"/>
     </row>
@@ -2326,7 +2323,7 @@
       <c r="H19" s="20">
         <v>1</v>
       </c>
-      <c r="I19" s="111"/>
+      <c r="I19" s="112"/>
       <c r="J19" s="2"/>
       <c r="K19" s="2"/>
     </row>
@@ -2353,7 +2350,7 @@
       <c r="H20" s="20">
         <v>1</v>
       </c>
-      <c r="I20" s="111"/>
+      <c r="I20" s="112"/>
       <c r="J20" s="2"/>
       <c r="K20" s="2"/>
     </row>
@@ -2380,7 +2377,7 @@
       <c r="H21" s="20">
         <v>1</v>
       </c>
-      <c r="I21" s="111"/>
+      <c r="I21" s="112"/>
       <c r="J21" s="2"/>
       <c r="K21" s="2"/>
     </row>
@@ -2407,7 +2404,7 @@
       <c r="H22" s="20">
         <v>1</v>
       </c>
-      <c r="I22" s="111"/>
+      <c r="I22" s="112"/>
       <c r="J22" s="2"/>
       <c r="K22" s="2"/>
     </row>
@@ -2434,7 +2431,7 @@
       <c r="H23" s="20">
         <v>1</v>
       </c>
-      <c r="I23" s="111"/>
+      <c r="I23" s="112"/>
       <c r="J23" s="2"/>
       <c r="K23" s="2"/>
     </row>
@@ -2515,7 +2512,7 @@
       <c r="H26" s="20">
         <v>1</v>
       </c>
-      <c r="I26" s="110" t="s">
+      <c r="I26" s="111" t="s">
         <v>73</v>
       </c>
       <c r="J26" s="2"/>
@@ -2541,10 +2538,10 @@
       <c r="G27" s="31">
         <v>45052</v>
       </c>
-      <c r="H27" s="33">
-        <v>0</v>
-      </c>
-      <c r="I27" s="111"/>
+      <c r="H27" s="20">
+        <v>1</v>
+      </c>
+      <c r="I27" s="112"/>
       <c r="J27" s="2"/>
       <c r="K27" s="2"/>
     </row>
@@ -2571,7 +2568,7 @@
       <c r="H28" s="33">
         <v>0</v>
       </c>
-      <c r="I28" s="110" t="s">
+      <c r="I28" s="111" t="s">
         <v>80</v>
       </c>
       <c r="J28" s="2"/>
@@ -2600,7 +2597,7 @@
       <c r="H29" s="33">
         <v>0</v>
       </c>
-      <c r="I29" s="111"/>
+      <c r="I29" s="112"/>
       <c r="J29" s="2"/>
       <c r="K29" s="2"/>
     </row>
@@ -2622,9 +2619,9 @@
       </c>
       <c r="H30" s="43">
         <f>SUM(H10:H29)/21</f>
-        <v>0.80952380952380953</v>
-      </c>
-      <c r="I30" s="111"/>
+        <v>0.8571428571428571</v>
+      </c>
+      <c r="I30" s="112"/>
     </row>
     <row r="31" spans="1:11" ht="15.75" customHeight="1" thickBot="1">
       <c r="A31" s="9"/>
@@ -2813,7 +2810,7 @@
       <c r="H37" s="54">
         <v>0</v>
       </c>
-      <c r="I37" s="110" t="s">
+      <c r="I37" s="111" t="s">
         <v>96</v>
       </c>
       <c r="J37" s="47"/>
@@ -2842,7 +2839,7 @@
       <c r="H38" s="54">
         <v>0</v>
       </c>
-      <c r="I38" s="111"/>
+      <c r="I38" s="112"/>
       <c r="J38" s="47"/>
       <c r="K38" s="2"/>
     </row>
@@ -2866,7 +2863,7 @@
         <f>SUM(H31:H38)/9</f>
         <v>0</v>
       </c>
-      <c r="I39" s="111"/>
+      <c r="I39" s="112"/>
     </row>
     <row r="40" spans="1:11" ht="15.75" customHeight="1" thickBot="1">
       <c r="A40" s="9"/>
@@ -3134,7 +3131,7 @@
       <c r="H49" s="54">
         <v>0</v>
       </c>
-      <c r="I49" s="110" t="s">
+      <c r="I49" s="111" t="s">
         <v>120</v>
       </c>
       <c r="J49" s="47"/>
@@ -3163,7 +3160,7 @@
       <c r="H50" s="54">
         <v>0</v>
       </c>
-      <c r="I50" s="111"/>
+      <c r="I50" s="112"/>
       <c r="J50" s="47"/>
       <c r="K50" s="2"/>
     </row>
@@ -3190,7 +3187,7 @@
       <c r="H51" s="54">
         <v>0</v>
       </c>
-      <c r="I51" s="110" t="s">
+      <c r="I51" s="111" t="s">
         <v>123</v>
       </c>
       <c r="J51" s="47"/>
@@ -3219,7 +3216,7 @@
       <c r="H52" s="54">
         <v>0</v>
       </c>
-      <c r="I52" s="111"/>
+      <c r="I52" s="112"/>
       <c r="J52" s="47"/>
       <c r="K52" s="2"/>
     </row>
@@ -3245,7 +3242,7 @@
         <f>SUM(H40:H52)/13</f>
         <v>0</v>
       </c>
-      <c r="I53" s="111"/>
+      <c r="I53" s="112"/>
     </row>
     <row r="54" spans="1:11" ht="15.75" customHeight="1">
       <c r="B54" s="22"/>
@@ -5049,10 +5046,10 @@
       <c r="C2" s="9"/>
     </row>
     <row r="3" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B3" s="115" t="s">
+      <c r="B3" s="116" t="s">
         <v>130</v>
       </c>
-      <c r="C3" s="116"/>
+      <c r="C3" s="117"/>
     </row>
     <row r="4" spans="2:3" ht="15.75" customHeight="1">
       <c r="B4" s="74" t="s">

</xml_diff>